<commit_message>
possible future design using a spherical bearing
</commit_message>
<xml_diff>
--- a/Design/Mechanik/vx/Gelenklager_Igus.xlsx
+++ b/Design/Mechanik/vx/Gelenklager_Igus.xlsx
@@ -125,12 +125,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,6 +163,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -468,7 +476,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,31 +622,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>12</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>18</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>11.1</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="6">
         <v>10.24</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="5" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>